<commit_message>
statistics for release 92
</commit_message>
<xml_diff>
--- a/intenz-database/src/site/resources/statistics/intenzStats-2013.xlsx
+++ b/intenz-database/src/site/resources/statistics/intenzStats-2013.xlsx
@@ -445,9 +445,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Table!$B$1:$N$1</c:f>
+              <c:f>Table!$B$1:$O$1</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>84</c:v>
                 </c:pt>
@@ -470,10 +470,10 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -485,6 +485,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -492,10 +495,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Table!$B$8:$N$8</c:f>
+              <c:f>Table!$B$8:$O$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>5022</c:v>
                 </c:pt>
@@ -518,10 +521,10 @@
                   <c:v>5191</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>5203</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>5204</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -533,6 +536,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -565,9 +571,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Table!$B$1:$N$1</c:f>
+              <c:f>Table!$B$1:$O$1</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>84</c:v>
                 </c:pt>
@@ -590,10 +596,10 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -605,6 +611,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -612,10 +621,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Table!$B$9:$N$9</c:f>
+              <c:f>Table!$B$9:$O$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>836</c:v>
                 </c:pt>
@@ -638,10 +647,10 @@
                   <c:v>863</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>863</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>863</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -653,6 +662,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -685,9 +697,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Table!$B$1:$N$1</c:f>
+              <c:f>Table!$B$1:$O$1</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>84</c:v>
                 </c:pt>
@@ -710,10 +722,10 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -725,6 +737,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -732,10 +747,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Table!$B$10:$N$10</c:f>
+              <c:f>Table!$B$10:$O$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>73</c:v>
                 </c:pt>
@@ -758,10 +773,10 @@
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -773,6 +788,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -805,9 +823,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Table!$B$1:$N$1</c:f>
+              <c:f>Table!$B$1:$O$1</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>84</c:v>
                 </c:pt>
@@ -830,10 +848,10 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -845,6 +863,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -852,10 +873,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Table!$B$11:$N$11</c:f>
+              <c:f>Table!$B$11:$O$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>111</c:v>
                 </c:pt>
@@ -878,10 +899,10 @@
                   <c:v>129</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>129</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>129</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -893,6 +914,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -925,9 +949,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Table!$B$1:$N$1</c:f>
+              <c:f>Table!$B$1:$O$1</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>84</c:v>
                 </c:pt>
@@ -950,10 +974,10 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -965,6 +989,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -972,10 +999,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Table!$B$12:$N$12</c:f>
+              <c:f>Table!$B$12:$O$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1013,6 +1040,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -1045,9 +1075,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Table!$B$1:$N$1</c:f>
+              <c:f>Table!$B$1:$O$1</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>84</c:v>
                 </c:pt>
@@ -1070,10 +1100,10 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -1085,6 +1115,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -1092,10 +1125,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Table!$B$13:$N$13</c:f>
+              <c:f>Table!$B$13:$O$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v/>
                 </c:pt>
@@ -1133,6 +1166,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -1165,9 +1201,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Table!$B$1:$N$1</c:f>
+              <c:f>Table!$B$1:$O$1</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>84</c:v>
                 </c:pt>
@@ -1190,10 +1226,10 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -1205,6 +1241,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -1212,10 +1251,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Table!$B$14:$N$14</c:f>
+              <c:f>Table!$B$14:$O$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>39</c:v>
                 </c:pt>
@@ -1238,10 +1277,10 @@
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -1253,6 +1292,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -1285,9 +1327,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Table!$B$1:$N$1</c:f>
+              <c:f>Table!$B$1:$O$1</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>84</c:v>
                 </c:pt>
@@ -1310,10 +1352,10 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -1325,6 +1367,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -1332,10 +1377,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Table!$B$15:$N$15</c:f>
+              <c:f>Table!$B$15:$O$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v/>
                 </c:pt>
@@ -1373,6 +1418,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -1381,11 +1429,11 @@
         </c:ser>
         <c:overlap val="100"/>
         <c:gapWidth val="100"/>
-        <c:axId val="92872724"/>
-        <c:axId val="59048945"/>
+        <c:axId val="70259507"/>
+        <c:axId val="8202478"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="92872724"/>
+        <c:axId val="70259507"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1419,14 +1467,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="59048945"/>
+        <c:crossAx val="8202478"/>
         <c:crossesAt val="3000"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="59048945"/>
+        <c:axId val="8202478"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="3000"/>
@@ -1475,7 +1523,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="92872724"/>
+        <c:crossAx val="70259507"/>
         <c:crosses val="min"/>
       </c:valAx>
       <c:spPr>
@@ -1556,9 +1604,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Table!$B$1:$N$1</c:f>
+              <c:f>Table!$B$1:$O$1</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>84</c:v>
                 </c:pt>
@@ -1581,10 +1629,10 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -1596,6 +1644,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -1603,10 +1654,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Table!$B$43:$N$43</c:f>
+              <c:f>Table!$B$43:$O$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>5858</c:v>
                 </c:pt>
@@ -1629,10 +1680,10 @@
                   <c:v>6054</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>6066</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>6067</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -1644,6 +1695,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1676,9 +1730,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Table!$B$1:$N$1</c:f>
+              <c:f>Table!$B$1:$O$1</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>84</c:v>
                 </c:pt>
@@ -1701,10 +1755,10 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -1716,6 +1770,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -1723,10 +1780,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Table!$B$44:$N$44</c:f>
+              <c:f>Table!$B$44:$O$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>184</c:v>
                 </c:pt>
@@ -1749,10 +1806,10 @@
                   <c:v>199</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>202</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -1764,6 +1821,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1796,9 +1856,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Table!$B$1:$N$1</c:f>
+              <c:f>Table!$B$1:$O$1</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>84</c:v>
                 </c:pt>
@@ -1821,10 +1881,10 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -1836,6 +1896,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -1843,10 +1906,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Table!$B$45:$N$45</c:f>
+              <c:f>Table!$B$45:$O$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1869,10 +1932,10 @@
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -1884,6 +1947,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1892,11 +1958,11 @@
         </c:ser>
         <c:overlap val="100"/>
         <c:gapWidth val="100"/>
-        <c:axId val="91152279"/>
-        <c:axId val="33491420"/>
+        <c:axId val="21469760"/>
+        <c:axId val="57982202"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="91152279"/>
+        <c:axId val="21469760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1930,14 +1996,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="33491420"/>
+        <c:crossAx val="57982202"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="33491420"/>
+        <c:axId val="57982202"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="4600"/>
@@ -1986,7 +2052,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="91152279"/>
+        <c:crossAx val="21469760"/>
         <c:crosses val="min"/>
         <c:majorUnit val="100"/>
         <c:minorUnit val="50"/>
@@ -2069,9 +2135,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Table!$B$1:$N$1</c:f>
+              <c:f>Table!$B$1:$O$1</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>84</c:v>
                 </c:pt>
@@ -2094,10 +2160,10 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -2109,6 +2175,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -2116,10 +2185,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Table!$B$27:$N$27</c:f>
+              <c:f>Table!$B$27:$O$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>3375</c:v>
                 </c:pt>
@@ -2142,10 +2211,10 @@
                   <c:v>3360</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>3359</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>3359</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -2157,6 +2226,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -2189,9 +2261,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Table!$B$1:$N$1</c:f>
+              <c:f>Table!$B$1:$O$1</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>84</c:v>
                 </c:pt>
@@ -2214,10 +2286,10 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -2229,6 +2301,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -2236,10 +2311,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Table!$B$28:$N$28</c:f>
+              <c:f>Table!$B$28:$O$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>96</c:v>
                 </c:pt>
@@ -2262,10 +2337,10 @@
                   <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -2277,6 +2352,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -2309,9 +2387,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Table!$B$1:$N$1</c:f>
+              <c:f>Table!$B$1:$O$1</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>84</c:v>
                 </c:pt>
@@ -2334,10 +2412,10 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -2349,6 +2427,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -2356,10 +2437,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Table!$B$29:$N$29</c:f>
+              <c:f>Table!$B$29:$O$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>344</c:v>
                 </c:pt>
@@ -2382,10 +2463,10 @@
                   <c:v>344</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>344</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>344</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -2397,6 +2478,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -2429,9 +2513,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Table!$B$1:$N$1</c:f>
+              <c:f>Table!$B$1:$O$1</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>84</c:v>
                 </c:pt>
@@ -2454,10 +2538,10 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -2469,6 +2553,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -2476,10 +2563,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Table!$B$30:$N$30</c:f>
+              <c:f>Table!$B$30:$O$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>352</c:v>
                 </c:pt>
@@ -2502,10 +2589,10 @@
                   <c:v>351</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>351</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>351</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -2517,6 +2604,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -2549,9 +2639,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Table!$B$1:$N$1</c:f>
+              <c:f>Table!$B$1:$O$1</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>84</c:v>
                 </c:pt>
@@ -2574,10 +2664,10 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -2589,6 +2679,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -2596,10 +2689,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Table!$B$31:$N$31</c:f>
+              <c:f>Table!$B$31:$O$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>218</c:v>
                 </c:pt>
@@ -2622,10 +2715,10 @@
                   <c:v>217</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>217</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>217</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -2637,6 +2730,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -2669,9 +2765,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Table!$B$1:$N$1</c:f>
+              <c:f>Table!$B$1:$O$1</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>84</c:v>
                 </c:pt>
@@ -2694,10 +2790,10 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -2709,6 +2805,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -2716,10 +2815,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Table!$B$32:$N$32</c:f>
+              <c:f>Table!$B$32:$O$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>710</c:v>
                 </c:pt>
@@ -2742,10 +2841,10 @@
                   <c:v>694</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>688</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>684</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -2757,6 +2856,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -2765,11 +2867,11 @@
         </c:ser>
         <c:overlap val="100"/>
         <c:gapWidth val="100"/>
-        <c:axId val="59352692"/>
-        <c:axId val="25075924"/>
+        <c:axId val="1663056"/>
+        <c:axId val="51863891"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="59352692"/>
+        <c:axId val="1663056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2808,14 +2910,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="25075924"/>
+        <c:crossAx val="51863891"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="25075924"/>
+        <c:axId val="51863891"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2863,7 +2965,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="59352692"/>
+        <c:crossAx val="1663056"/>
         <c:crosses val="min"/>
       </c:valAx>
       <c:spPr>
@@ -2944,9 +3046,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Table!$B$1:$N$1</c:f>
+              <c:f>Table!$B$1:$O$1</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>84</c:v>
                 </c:pt>
@@ -2969,10 +3071,10 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -2984,6 +3086,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -2991,10 +3096,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Table!$B$25:$N$25</c:f>
+              <c:f>Table!$B$25:$O$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>208827</c:v>
                 </c:pt>
@@ -3017,10 +3122,10 @@
                   <c:v>210037</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>210041</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>212487</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -3032,6 +3137,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -3064,9 +3172,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Table!$B$1:$N$1</c:f>
+              <c:f>Table!$B$1:$O$1</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>84</c:v>
                 </c:pt>
@@ -3089,10 +3197,10 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -3104,6 +3212,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -3111,10 +3222,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Table!$B$23:$N$23</c:f>
+              <c:f>Table!$B$23:$O$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>3975</c:v>
                 </c:pt>
@@ -3137,10 +3248,10 @@
                   <c:v>3962</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>3962</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>3962</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -3152,6 +3263,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -3184,9 +3298,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Table!$B$1:$N$1</c:f>
+              <c:f>Table!$B$1:$O$1</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>84</c:v>
                 </c:pt>
@@ -3209,10 +3323,10 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -3224,6 +3338,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -3231,10 +3348,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Table!$B$24:$N$24</c:f>
+              <c:f>Table!$B$24:$O$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>466</c:v>
                 </c:pt>
@@ -3257,10 +3374,10 @@
                   <c:v>466</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>466</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>466</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -3272,6 +3389,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -3304,9 +3424,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Table!$B$1:$N$1</c:f>
+              <c:f>Table!$B$1:$O$1</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>84</c:v>
                 </c:pt>
@@ -3329,10 +3449,10 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -3344,6 +3464,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -3351,10 +3474,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Table!$B$22:$N$22</c:f>
+              <c:f>Table!$B$22:$O$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>544</c:v>
                 </c:pt>
@@ -3377,10 +3500,10 @@
                   <c:v>552</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>552</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>552</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -3392,6 +3515,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -3400,11 +3526,11 @@
         </c:ser>
         <c:overlap val="100"/>
         <c:gapWidth val="100"/>
-        <c:axId val="28841590"/>
-        <c:axId val="98766775"/>
+        <c:axId val="86147800"/>
+        <c:axId val="90493366"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="28841590"/>
+        <c:axId val="86147800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3420,14 +3546,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="98766775"/>
+        <c:crossAx val="90493366"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98766775"/>
+        <c:axId val="90493366"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="160000"/>
@@ -3476,7 +3602,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="28841590"/>
+        <c:crossAx val="86147800"/>
         <c:crosses val="min"/>
       </c:valAx>
       <c:spPr>
@@ -3557,9 +3683,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Table!$B$1:$N$1</c:f>
+              <c:f>Table!$B$1:$O$1</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>84</c:v>
                 </c:pt>
@@ -3582,10 +3708,10 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -3597,6 +3723,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -3604,10 +3733,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Table!$B$20:$N$20</c:f>
+              <c:f>Table!$B$20:$O$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>219639</c:v>
                 </c:pt>
@@ -3630,10 +3759,10 @@
                   <c:v>221105</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>221109</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>224018</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -3645,6 +3774,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -3677,9 +3809,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Table!$B$1:$N$1</c:f>
+              <c:f>Table!$B$1:$O$1</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>84</c:v>
                 </c:pt>
@@ -3702,10 +3834,10 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -3717,6 +3849,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -3724,10 +3859,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Table!$B$18:$N$18</c:f>
+              <c:f>Table!$B$18:$O$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>4002</c:v>
                 </c:pt>
@@ -3750,10 +3885,10 @@
                   <c:v>3988</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>3988</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>3988</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -3765,6 +3900,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -3797,9 +3935,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Table!$B$1:$N$1</c:f>
+              <c:f>Table!$B$1:$O$1</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>84</c:v>
                 </c:pt>
@@ -3822,10 +3960,10 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -3837,6 +3975,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -3844,10 +3985,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Table!$B$19:$N$19</c:f>
+              <c:f>Table!$B$19:$O$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1442</c:v>
                 </c:pt>
@@ -3870,10 +4011,10 @@
                   <c:v>1442</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>1442</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>1442</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -3885,6 +4026,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -3917,9 +4061,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Table!$B$1:$N$1</c:f>
+              <c:f>Table!$B$1:$O$1</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>84</c:v>
                 </c:pt>
@@ -3942,10 +4086,10 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -3957,6 +4101,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -3964,10 +4111,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Table!$B$17:$N$17</c:f>
+              <c:f>Table!$B$17:$O$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1690</c:v>
                 </c:pt>
@@ -3990,10 +4137,10 @@
                   <c:v>1711</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>1711</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>1711</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -4005,6 +4152,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -4013,11 +4163,11 @@
         </c:ser>
         <c:overlap val="100"/>
         <c:gapWidth val="100"/>
-        <c:axId val="64817583"/>
-        <c:axId val="23305296"/>
+        <c:axId val="91672731"/>
+        <c:axId val="90793596"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="64817583"/>
+        <c:axId val="91672731"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4033,14 +4183,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="23305296"/>
+        <c:crossAx val="90793596"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="23305296"/>
+        <c:axId val="90793596"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="160000"/>
@@ -4089,7 +4239,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="64817583"/>
+        <c:crossAx val="91672731"/>
         <c:crosses val="min"/>
       </c:valAx>
       <c:spPr>
@@ -4144,9 +4294,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Table!$A$1:$N$1</c:f>
+              <c:f>Table!$A$1:$O$1</c:f>
               <c:strCache>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>Release number</c:v>
                 </c:pt>
@@ -4172,10 +4322,10 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v/>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v/>
@@ -4187,6 +4337,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="13">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v/>
                 </c:pt>
               </c:strCache>
@@ -4194,10 +4347,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Table!$A$6:$N$6</c:f>
+              <c:f>Table!$A$6:$O$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v/>
                 </c:pt>
@@ -4223,10 +4376,10 @@
                   <c:v>19844</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>19877</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v/>
+                  <c:v>19889</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v/>
@@ -4238,6 +4391,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="13">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -4245,11 +4401,11 @@
           </c:val>
         </c:ser>
         <c:marker val="0"/>
-        <c:axId val="26271008"/>
-        <c:axId val="41157330"/>
+        <c:axId val="84655267"/>
+        <c:axId val="71784288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="26271008"/>
+        <c:axId val="84655267"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4288,14 +4444,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="41157330"/>
+        <c:crossAx val="71784288"/>
         <c:crossesAt val="17000"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="41157330"/>
+        <c:axId val="71784288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -4344,7 +4500,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="26271008"/>
+        <c:crossAx val="84655267"/>
         <c:crosses val="min"/>
       </c:valAx>
       <c:spPr>
@@ -4370,13 +4526,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>165600</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>2160</xdr:rowOff>
+      <xdr:rowOff>2520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>83880</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>6480</xdr:rowOff>
+      <xdr:rowOff>1080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4384,8 +4540,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="165600" y="161280"/>
-        <a:ext cx="11590200" cy="3839040"/>
+        <a:off x="165600" y="161640"/>
+        <a:ext cx="11590200" cy="3833280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4400,7 +4556,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>152280</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>88920</xdr:rowOff>
+      <xdr:rowOff>89280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
@@ -4414,8 +4570,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="152280" y="4082760"/>
-        <a:ext cx="11638800" cy="3739680"/>
+        <a:off x="152280" y="4083120"/>
+        <a:ext cx="11638800" cy="3739320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4474,9 +4630,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>491760</xdr:colOff>
+      <xdr:colOff>495720</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>144000</xdr:rowOff>
+      <xdr:rowOff>141480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4485,7 +4641,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="292680" y="19440"/>
-        <a:ext cx="11245320" cy="3661200"/>
+        <a:ext cx="11249280" cy="3658680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4500,13 +4656,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>318600</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>148320</xdr:rowOff>
+      <xdr:rowOff>148680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>522000</xdr:colOff>
+      <xdr:colOff>525960</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>91080</xdr:rowOff>
+      <xdr:rowOff>91800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4514,8 +4670,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="318600" y="3844440"/>
-        <a:ext cx="11249640" cy="3768120"/>
+        <a:off x="318600" y="3844800"/>
+        <a:ext cx="11253600" cy="3768480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4568,13 +4724,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N45"/>
+  <dimension ref="A1:O45"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="H3" activeCellId="0" pane="topLeft" sqref="H3"/>
+      <selection activeCell="K1" activeCellId="0" pane="topLeft" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.55"/>
+  <sheetFormatPr defaultRowHeight="12.1"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.7633928571429"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.4419642857143"/>
@@ -4605,6 +4761,12 @@
       <c r="H1" s="1" t="n">
         <v>90</v>
       </c>
+      <c r="I1" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>92</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="1" t="s">
@@ -4631,12 +4793,17 @@
       <c r="H2" s="2" t="n">
         <v>41492</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
+      <c r="I2" s="2" t="n">
+        <v>41521</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>41563</v>
+      </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="A3" s="1" t="s">
@@ -4663,6 +4830,12 @@
       <c r="H3" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="I3" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="1" t="s">
@@ -4689,8 +4862,14 @@
       <c r="H4" s="0" t="n">
         <v>69</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="5">
+      <c r="I4" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="5">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -4715,8 +4894,14 @@
       <c r="H5" s="3" t="n">
         <v>287</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="6">
+      <c r="I5" s="3" t="n">
+        <v>287</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>287</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="6">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -4740,6 +4925,12 @@
       </c>
       <c r="H6" s="3" t="n">
         <v>19844</v>
+      </c>
+      <c r="I6" s="3" t="n">
+        <v>19877</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>19889</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
@@ -4748,8 +4939,9 @@
       </c>
       <c r="B7" s="4"/>
       <c r="H7" s="3"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="8">
+      <c r="I7" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.25" outlineLevel="0" r="8">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -4773,6 +4965,12 @@
       </c>
       <c r="H8" s="3" t="n">
         <v>5191</v>
+      </c>
+      <c r="I8" s="3" t="n">
+        <v>5203</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>5204</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
@@ -4800,6 +4998,12 @@
       <c r="H9" s="0" t="n">
         <v>863</v>
       </c>
+      <c r="I9" s="0" t="n">
+        <v>863</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>863</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="A10" s="4" t="s">
@@ -4826,6 +5030,12 @@
       <c r="H10" s="0" t="n">
         <v>70</v>
       </c>
+      <c r="I10" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>73</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
       <c r="A11" s="4" t="s">
@@ -4852,6 +5062,12 @@
       <c r="H11" s="0" t="n">
         <v>129</v>
       </c>
+      <c r="I11" s="0" t="n">
+        <v>129</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>129</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
       <c r="A12" s="4" t="s">
@@ -4894,6 +5110,12 @@
       <c r="H14" s="0" t="n">
         <v>18</v>
       </c>
+      <c r="I14" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>64</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
       <c r="A15" s="4" t="s">
@@ -4930,6 +5152,12 @@
       <c r="H17" s="0" t="n">
         <v>1711</v>
       </c>
+      <c r="I17" s="0" t="n">
+        <v>1711</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>1711</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
       <c r="A18" s="4" t="s">
@@ -4956,6 +5184,12 @@
       <c r="H18" s="0" t="n">
         <v>3988</v>
       </c>
+      <c r="I18" s="0" t="n">
+        <v>3988</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <v>3988</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
       <c r="A19" s="4" t="s">
@@ -4982,6 +5216,12 @@
       <c r="H19" s="0" t="n">
         <v>1442</v>
       </c>
+      <c r="I19" s="0" t="n">
+        <v>1442</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <v>1442</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
       <c r="A20" s="4" t="s">
@@ -5008,6 +5248,12 @@
       <c r="H20" s="0" t="n">
         <v>221105</v>
       </c>
+      <c r="I20" s="0" t="n">
+        <v>221109</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <v>224018</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
       <c r="A21" s="1" t="s">
@@ -5039,6 +5285,12 @@
       <c r="H22" s="0" t="n">
         <v>552</v>
       </c>
+      <c r="I22" s="0" t="n">
+        <v>552</v>
+      </c>
+      <c r="J22" s="0" t="n">
+        <v>552</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
       <c r="A23" s="4" t="s">
@@ -5065,6 +5317,12 @@
       <c r="H23" s="0" t="n">
         <v>3962</v>
       </c>
+      <c r="I23" s="0" t="n">
+        <v>3962</v>
+      </c>
+      <c r="J23" s="0" t="n">
+        <v>3962</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
       <c r="A24" s="4" t="s">
@@ -5091,6 +5349,12 @@
       <c r="H24" s="0" t="n">
         <v>466</v>
       </c>
+      <c r="I24" s="0" t="n">
+        <v>466</v>
+      </c>
+      <c r="J24" s="0" t="n">
+        <v>466</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
       <c r="A25" s="4" t="s">
@@ -5117,6 +5381,12 @@
       <c r="H25" s="0" t="n">
         <v>210037</v>
       </c>
+      <c r="I25" s="0" t="n">
+        <v>210041</v>
+      </c>
+      <c r="J25" s="0" t="n">
+        <v>212487</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
       <c r="A26" s="1" t="s">
@@ -5148,6 +5418,12 @@
       <c r="H27" s="0" t="n">
         <v>3360</v>
       </c>
+      <c r="I27" s="0" t="n">
+        <v>3359</v>
+      </c>
+      <c r="J27" s="0" t="n">
+        <v>3359</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
       <c r="A28" s="4" t="s">
@@ -5174,6 +5450,12 @@
       <c r="H28" s="0" t="n">
         <v>110</v>
       </c>
+      <c r="I28" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="J28" s="0" t="n">
+        <v>120</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
       <c r="A29" s="4" t="s">
@@ -5200,6 +5482,12 @@
       <c r="H29" s="0" t="n">
         <v>344</v>
       </c>
+      <c r="I29" s="0" t="n">
+        <v>344</v>
+      </c>
+      <c r="J29" s="0" t="n">
+        <v>344</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
       <c r="A30" s="4" t="s">
@@ -5226,6 +5514,12 @@
       <c r="H30" s="0" t="n">
         <v>351</v>
       </c>
+      <c r="I30" s="0" t="n">
+        <v>351</v>
+      </c>
+      <c r="J30" s="0" t="n">
+        <v>351</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="31">
       <c r="A31" s="4" t="s">
@@ -5252,6 +5546,12 @@
       <c r="H31" s="0" t="n">
         <v>217</v>
       </c>
+      <c r="I31" s="0" t="n">
+        <v>217</v>
+      </c>
+      <c r="J31" s="0" t="n">
+        <v>217</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
       <c r="A32" s="4" t="s">
@@ -5278,6 +5578,12 @@
       <c r="H32" s="0" t="n">
         <v>694</v>
       </c>
+      <c r="I32" s="0" t="n">
+        <v>688</v>
+      </c>
+      <c r="J32" s="0" t="n">
+        <v>684</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33">
       <c r="A33" s="1" t="s">
@@ -5309,6 +5615,12 @@
       <c r="H34" s="0" t="n">
         <v>3193</v>
       </c>
+      <c r="I34" s="0" t="n">
+        <v>3193</v>
+      </c>
+      <c r="J34" s="0" t="n">
+        <v>3193</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="35">
       <c r="A35" s="4" t="s">
@@ -5335,6 +5647,12 @@
       <c r="H35" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="I35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J35" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="36">
       <c r="A36" s="4" t="s">
@@ -5361,6 +5679,12 @@
       <c r="H36" s="0" t="n">
         <v>337</v>
       </c>
+      <c r="I36" s="0" t="n">
+        <v>337</v>
+      </c>
+      <c r="J36" s="0" t="n">
+        <v>337</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="37">
       <c r="A37" s="4" t="s">
@@ -5387,6 +5711,12 @@
       <c r="H37" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="I37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J37" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="38">
       <c r="A38" s="4" t="s">
@@ -5413,6 +5743,12 @@
       <c r="H38" s="0" t="n">
         <v>74</v>
       </c>
+      <c r="I38" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="J38" s="0" t="n">
+        <v>74</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="39">
       <c r="A39" s="4" t="s">
@@ -5439,22 +5775,28 @@
       <c r="H39" s="0" t="n">
         <v>641</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="40">
+      <c r="I39" s="0" t="n">
+        <v>635</v>
+      </c>
+      <c r="J39" s="0" t="n">
+        <v>631</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="40">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="41">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="41">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="42">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="42">
       <c r="A42" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B42" s="1"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="43" s="4">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="43" s="4">
       <c r="A43" s="4" t="s">
         <v>30</v>
       </c>
@@ -5488,11 +5830,11 @@
       </c>
       <c r="I43" s="4" t="n">
         <f aca="false">SUM(I8:I9)</f>
-        <v>0</v>
+        <v>6066</v>
       </c>
       <c r="J43" s="4" t="n">
         <f aca="false">SUM(J8:J9)</f>
-        <v>0</v>
+        <v>6067</v>
       </c>
       <c r="K43" s="4" t="n">
         <f aca="false">SUM(K8:K9)</f>
@@ -5510,8 +5852,12 @@
         <f aca="false">SUM(N8:N9)</f>
         <v>0</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="44" s="4">
+      <c r="O43" s="4" t="n">
+        <f aca="false">SUM(O8:O9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="44" s="4">
       <c r="A44" s="4" t="s">
         <v>31</v>
       </c>
@@ -5545,11 +5891,11 @@
       </c>
       <c r="I44" s="4" t="n">
         <f aca="false">SUM(I10:I11)</f>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="J44" s="4" t="n">
         <f aca="false">SUM(J10:J11)</f>
-        <v>0</v>
+        <v>202</v>
       </c>
       <c r="K44" s="4" t="n">
         <f aca="false">SUM(K10:K11)</f>
@@ -5567,8 +5913,12 @@
         <f aca="false">SUM(N10:N11)</f>
         <v>0</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="45" s="4">
+      <c r="O44" s="4" t="n">
+        <f aca="false">SUM(O10:O11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="45" s="4">
       <c r="A45" s="4" t="s">
         <v>32</v>
       </c>
@@ -5601,12 +5951,12 @@
         <v>18</v>
       </c>
       <c r="I45" s="4" t="n">
-        <f aca="false">I12</f>
-        <v>0</v>
+        <f aca="false">I14</f>
+        <v>3</v>
       </c>
       <c r="J45" s="4" t="n">
-        <f aca="false">J12</f>
-        <v>0</v>
+        <f aca="false">J14</f>
+        <v>64</v>
       </c>
       <c r="K45" s="4" t="n">
         <f aca="false">K12</f>
@@ -5624,11 +5974,15 @@
         <f aca="false">N12</f>
         <v>0</v>
       </c>
+      <c r="O45" s="4" t="n">
+        <f aca="false">O12</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Arial,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Arial,Regular"Page &amp;P</oddFooter>
@@ -5851,7 +6205,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -5889,7 +6243,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -5925,7 +6279,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -5967,7 +6321,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>